<commit_message>
Removed extra sheets in farmer import templates
</commit_message>
<xml_diff>
--- a/src/assets/farmer-import/Plantilla_listado de agricultores_es.xlsx
+++ b/src/assets/farmer-import/Plantilla_listado de agricultores_es.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0587f98c1ebf2769/Freelance/Aufträge/giz 2022-2023/Implementacion HON cafe/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pecea/WebstormProjects/INATRACE/inatrace-fe/src/assets/farmer-import/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{4C768EF3-87B3-6242-8F0D-6D2A12F8EB44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{588FE5E5-1333-664E-AB3E-EA02FA71B74F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F2989A-FC48-B04A-B108-E0443F299DA9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -356,12 +354,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection hidden="1"/>
@@ -381,10 +373,16 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{689D75BB-9489-7241-AE71-B16908EB7EFB}"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
@@ -1620,11 +1618,11 @@
     <row r="2" spans="1:40" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -1729,10 +1727,10 @@
       <c r="W4" s="7"/>
       <c r="X4" s="7"/>
       <c r="Y4" s="7"/>
-      <c r="Z4" s="22" t="s">
+      <c r="Z4" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="AA4" s="22" t="s">
+      <c r="AA4" s="20" t="s">
         <v>34</v>
       </c>
       <c r="AB4" s="7"/>
@@ -1750,102 +1748,102 @@
       <c r="AN4" s="3"/>
     </row>
     <row r="5" spans="1:40" ht="64" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="22" t="s">
+      <c r="G5" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="22" t="s">
+      <c r="H5" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="22" t="s">
+      <c r="I5" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="22" t="s">
+      <c r="J5" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="23" t="s">
+      <c r="K5" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="23" t="s">
+      <c r="L5" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="23" t="s">
+      <c r="M5" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="N5" s="23" t="s">
+      <c r="N5" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="O5" s="22" t="s">
+      <c r="O5" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="P5" s="22" t="s">
+      <c r="P5" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="Q5" s="24" t="s">
+      <c r="Q5" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="R5" s="22" t="s">
+      <c r="R5" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="S5" s="22" t="s">
+      <c r="S5" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="T5" s="22" t="s">
+      <c r="T5" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="U5" s="23" t="s">
+      <c r="U5" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="V5" s="22" t="s">
+      <c r="V5" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="W5" s="22" t="s">
+      <c r="W5" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="X5" s="22" t="s">
+      <c r="X5" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="Y5" s="22" t="s">
+      <c r="Y5" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="Z5" s="25"/>
-      <c r="AA5" s="25"/>
-      <c r="AB5" s="22" t="s">
+      <c r="Z5" s="23"/>
+      <c r="AA5" s="23"/>
+      <c r="AB5" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="AC5" s="22" t="s">
+      <c r="AC5" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="AD5" s="22" t="s">
+      <c r="AD5" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="AE5" s="26" t="s">
+      <c r="AE5" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="AF5" s="26" t="s">
+      <c r="AF5" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="AG5" s="26" t="s">
+      <c r="AG5" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="AH5" s="26" t="s">
+      <c r="AH5" s="24" t="s">
         <v>31</v>
       </c>
       <c r="AI5" s="9"/>
@@ -12575,186 +12573,4 @@
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E10"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="6" width="8.6640625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.6640625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E10"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="6" width="8.6640625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.6640625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>